<commit_message>
Updated percent_income_yes function in income_pipeline
</commit_message>
<xml_diff>
--- a/BoSClean/Percent Income Entry & Exit.xlsx
+++ b/BoSClean/Percent Income Entry & Exit.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,14 +453,105 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>OC</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="C2" t="n">
+        <v>4.97</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>MC</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>5.43</v>
+      </c>
+      <c r="C3" t="n">
+        <v>5.69</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>SPC</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B4" t="n">
         <v>6.58</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C4" t="n">
         <v>23.4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>8319</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Erin</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="C7" t="n">
+        <v>4.95</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>11495</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>10.53</v>
+      </c>
+      <c r="C8" t="n">
+        <v>30.77</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>1371</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>3.01</v>
+      </c>
+      <c r="C9" t="n">
+        <v>5.21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>